<commit_message>
Update XLSX example to v0.0.4.
</commit_message>
<xml_diff>
--- a/examples/Tock Burn Document Example Template.xlsx
+++ b/examples/Tock Burn Document Example Template.xlsx
@@ -9,8 +9,11 @@
   </sheets>
   <definedNames>
     <definedName name="TOCK_API_KEY">Settings!$B$3:$C$3</definedName>
+    <definedName name="BurnDoc_avgRate">'Burn Sheet'!$C$4</definedName>
     <definedName name="GradeRates">Settings!$B$12:$C$18</definedName>
     <definedName name="PROJECT_PREFIX_FILTER">Settings!$B$6:$C$6</definedName>
+    <definedName name="BurnDoc_budget">'Burn Sheet'!$B$3</definedName>
+    <definedName name="BurnDoc_project">'Burn Sheet'!$B$1</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
@@ -706,21 +709,21 @@
         <v>32.0</v>
       </c>
       <c r="E8">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A8, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A8, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>28</v>
       </c>
       <c r="F8" s="10">
         <v>32.0</v>
       </c>
       <c r="G8">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A8, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A8, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H8" s="10">
         <v>32.0</v>
       </c>
       <c r="I8">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A8, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A8, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="AF8" s="19"/>
@@ -754,21 +757,21 @@
         <v>32.0</v>
       </c>
       <c r="E9">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A9, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A9, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>26</v>
       </c>
       <c r="F9" s="10">
         <v>32.0</v>
       </c>
       <c r="G9">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A9, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A9, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H9" s="10">
         <v>32.0</v>
       </c>
       <c r="I9">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A9, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A9, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="AF9" s="19"/>
@@ -802,21 +805,21 @@
         <v>32.0</v>
       </c>
       <c r="E10">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A10, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A10, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>29</v>
       </c>
       <c r="F10" s="10">
         <v>32.0</v>
       </c>
       <c r="G10">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A10, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A10, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H10" s="10">
         <v>32.0</v>
       </c>
       <c r="I10">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A10, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A10, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="AF10" s="19"/>
@@ -850,21 +853,21 @@
         <v>32.0</v>
       </c>
       <c r="E11">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A11, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A11, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>32</v>
       </c>
       <c r="F11" s="10">
         <v>32.0</v>
       </c>
       <c r="G11">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A11, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A11, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H11" s="10">
         <v>32.0</v>
       </c>
       <c r="I11">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A11, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A11, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="AF11" s="19"/>
@@ -898,21 +901,21 @@
         <v>32.0</v>
       </c>
       <c r="E12">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A12, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$B$1:$B992, $A12, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>32</v>
       </c>
       <c r="F12" s="10">
         <v>32.0</v>
       </c>
       <c r="G12">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A12, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$B$1:$B992, $A12, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H12" s="10">
         <v>32.0</v>
       </c>
       <c r="I12">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A12, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$B$1:$B992, $A12, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="J12" s="25"/>
@@ -1036,7 +1039,7 @@
         <v>160</v>
       </c>
       <c r="E16" s="29">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, D$6, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>177</v>
       </c>
       <c r="F16">
@@ -1044,7 +1047,7 @@
         <v>160</v>
       </c>
       <c r="G16" s="29">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, F$6, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -1052,7 +1055,7 @@
         <v>160</v>
       </c>
       <c r="I16" s="29">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$A$1:$A992, H$6, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="J16" s="25"/>
@@ -1084,27 +1087,27 @@
         <v>49</v>
       </c>
       <c r="D17" s="30">
-        <f>$C$4 * D16</f>
+        <f>BurnDoc_avgRate * D16</f>
         <v>6400</v>
       </c>
       <c r="E17" s="30">
-        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, D$6, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, D$6, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>6300</v>
       </c>
       <c r="F17" s="30">
-        <f>$C$4 * F16</f>
+        <f>BurnDoc_avgRate * F16</f>
         <v>6400</v>
       </c>
       <c r="G17" s="30">
-        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, F$6, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, F$6, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="H17" s="30">
-        <f>$C$4 * H16</f>
+        <f>BurnDoc_avgRate * H16</f>
         <v>6400</v>
       </c>
       <c r="I17" s="30">
-        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, H$6, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, H$6, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>0</v>
       </c>
       <c r="J17" s="25"/>
@@ -1136,7 +1139,7 @@
         <v>50</v>
       </c>
       <c r="C18" s="31">
-        <f>B3</f>
+        <f>BurnDoc_budget</f>
         <v>50000</v>
       </c>
       <c r="D18" s="31">
@@ -1144,7 +1147,7 @@
         <v>43600</v>
       </c>
       <c r="E18" s="31">
-        <f>IF(E17=0, "", $B$3 - SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, "&lt;=" &amp; D$6, Timecards!$C$1:$C992, $B$1))</f>
+        <f>IF(E17=0, "", $B$3 - SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, "&lt;=" &amp; D$6, Timecards!$C$1:$C992, BurnDoc_project))</f>
         <v>43700</v>
       </c>
       <c r="F18" s="31">
@@ -1152,7 +1155,7 @@
         <v>37300</v>
       </c>
       <c r="G18" t="str">
-        <f>IF(G17=0, "", $B$3 - SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, "&lt;=" &amp; F$6, Timecards!$C$1:$C992, $B$1))</f>
+        <f>IF(G17=0, "", $B$3 - SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, "&lt;=" &amp; F$6, Timecards!$C$1:$C992, BurnDoc_project))</f>
         <v/>
       </c>
       <c r="H18" s="31">
@@ -1160,7 +1163,7 @@
         <v>30900</v>
       </c>
       <c r="I18" t="str">
-        <f>IF(I17=0, "", $B$3 - SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, "&lt;=" &amp; H$6, Timecards!$C$1:$C992, $B$1))</f>
+        <f>IF(I17=0, "", $B$3 - SUMIFS(Timecards!$F$1:$F992, Timecards!$A$1:$A992, "&lt;=" &amp; H$6, Timecards!$C$1:$C992, BurnDoc_project))</f>
         <v/>
       </c>
       <c r="J18" s="25"/>
@@ -1245,7 +1248,7 @@
         <v>52</v>
       </c>
       <c r="B21">
-        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>177</v>
       </c>
       <c r="AH21" s="19"/>
@@ -1298,7 +1301,7 @@
         <v>53</v>
       </c>
       <c r="B23" s="32">
-        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$C$1:$C992, $B$1)</f>
+        <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$C$1:$C992, BurnDoc_project)</f>
         <v>6300</v>
       </c>
       <c r="AH23" s="19"/>
@@ -1328,7 +1331,7 @@
         <v>54</v>
       </c>
       <c r="B24" s="32">
-        <f>$B$3 - $B$23</f>
+        <f>BurnDoc_budget - $B$23</f>
         <v>43700</v>
       </c>
       <c r="AH24" s="19"/>
@@ -1460,7 +1463,7 @@
         <v>57</v>
       </c>
       <c r="B29" s="33" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("listDifferences($A$8:$A$15, UNIQUE(FILTER(Timecards!$B$1:$B992,Timecards!$C$1:$C992=$B$1)))"),"abraham.lincoln")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("listDifferences($A$8:$A$15, UNIQUE(FILTER(Timecards!$B$1:$B992,Timecards!$C$1:$C992=BurnDoc_project)))"),"abraham.lincoln")</f>
         <v>abraham.lincoln</v>
       </c>
       <c r="F29" s="33"/>
@@ -1553,7 +1556,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="33" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("listDifferences($B$6:$ABB$6, UNIQUE(FILTER(Timecards!$A$1:$A992,Timecards!$C$1:$C992=$B$1)))"),"")</f>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("listDifferences($B$6:$ABB$6, UNIQUE(FILTER(Timecards!$A$1:$A992,Timecards!$C$1:$C992=BurnDoc_project)))"),"")</f>
         <v/>
       </c>
       <c r="F32" s="33"/>
@@ -23665,16 +23668,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J6:K11"/>
+    <mergeCell ref="BA6:BB11"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B1:E1"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:C33"/>
-    <mergeCell ref="J6:K11"/>
-    <mergeCell ref="BA6:BB11"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -24118,15 +24121,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:C4"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C24"/>

</xml_diff>

<commit_message>
Update XLSX e xample to v0.0.5.
</commit_message>
<xml_diff>
--- a/examples/Tock Burn Document Example Template.xlsx
+++ b/examples/Tock Burn Document Example Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>start_date</t>
   </si>
@@ -151,10 +151,7 @@
     <t>Project participants</t>
   </si>
   <si>
-    <t>Copy and paste the previous two columns here and adjust the date to add more weeks to the project.</t>
-  </si>
-  <si>
-    <t>Feel free to add columns past this point.</t>
+    <t>Copy and paste the previous two columns here to add more weeks to the project.</t>
   </si>
   <si>
     <t>Est</t>
@@ -623,10 +620,12 @@
         <v>43037.0</v>
       </c>
       <c r="F6" s="24">
-        <v>43044.0</v>
+        <f>D6+7</f>
+        <v>43044</v>
       </c>
       <c r="H6" s="24">
-        <v>43051.0</v>
+        <f>F6+7</f>
+        <v>43051</v>
       </c>
       <c r="J6" s="25" t="s">
         <v>43</v>
@@ -652,31 +651,30 @@
       <c r="AX6" s="19"/>
       <c r="AY6" s="19"/>
       <c r="AZ6" s="19"/>
-      <c r="BA6" s="25" t="s">
-        <v>44</v>
-      </c>
+      <c r="BA6" s="25"/>
+      <c r="BB6" s="25"/>
     </row>
     <row r="7">
       <c r="A7" s="26"/>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
       <c r="D7" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="27" t="s">
-        <v>46</v>
+      <c r="F7" s="27" t="s">
+        <v>44</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="G7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="27" t="s">
-        <v>46</v>
-      </c>
       <c r="H7" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AF7" s="19"/>
       <c r="AG7" s="19"/>
@@ -699,6 +697,8 @@
       <c r="AX7" s="19"/>
       <c r="AY7" s="19"/>
       <c r="AZ7" s="19"/>
+      <c r="BA7" s="25"/>
+      <c r="BB7" s="25"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
@@ -747,6 +747,8 @@
       <c r="AX8" s="19"/>
       <c r="AY8" s="19"/>
       <c r="AZ8" s="19"/>
+      <c r="BA8" s="25"/>
+      <c r="BB8" s="25"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
@@ -795,6 +797,8 @@
       <c r="AX9" s="19"/>
       <c r="AY9" s="19"/>
       <c r="AZ9" s="19"/>
+      <c r="BA9" s="25"/>
+      <c r="BB9" s="25"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
@@ -843,6 +847,8 @@
       <c r="AX10" s="19"/>
       <c r="AY10" s="19"/>
       <c r="AZ10" s="19"/>
+      <c r="BA10" s="25"/>
+      <c r="BB10" s="25"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
@@ -891,6 +897,8 @@
       <c r="AX11" s="19"/>
       <c r="AY11" s="19"/>
       <c r="AZ11" s="19"/>
+      <c r="BA11" s="25"/>
+      <c r="BB11" s="25"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
@@ -974,7 +982,7 @@
     </row>
     <row r="14" ht="57.0">
       <c r="A14" s="28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="10"/>
       <c r="D14" s="10"/>
@@ -1031,7 +1039,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16">
@@ -1084,7 +1092,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" s="30">
         <f>BurnDoc_avgRate * D16</f>
@@ -1136,7 +1144,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="31">
         <f>BurnDoc_budget</f>
@@ -1215,7 +1223,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20">
         <f>SUMPRODUCT(--(MOD(COLUMN($B$16:BB$16),2)=0),$B$16:BB$16)</f>
@@ -1245,7 +1253,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <f>SUMIFS(Timecards!$D$1:$D992, Timecards!$C$1:$C992, BurnDoc_project)</f>
@@ -1298,7 +1306,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="32">
         <f>SUMIFS(Timecards!$F$1:$F992, Timecards!$C$1:$C992, BurnDoc_project)</f>
@@ -1328,7 +1336,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="32">
         <f>BurnDoc_budget - $B$23</f>
@@ -1358,7 +1366,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="32">
         <f>IFERROR(__xludf.DUMMYFUNCTION("INDEX(FILTER($C$18:BB$18, $C$18:BB$18 &lt;&gt; """"), 1, COUNTA(FILTER($C$18:BB$18, $C$18:BB$18 &lt;&gt; """")))"),"$30,900.00")</f>
@@ -1411,7 +1419,7 @@
     </row>
     <row r="27" ht="21.0">
       <c r="A27" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AH27" s="19"/>
       <c r="AI27" s="19"/>
@@ -1460,7 +1468,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" s="33" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("listDifferences($A$8:$A$15, UNIQUE(FILTER(Timecards!$B$1:$B992,Timecards!$C$1:$C992=BurnDoc_project)))"),"abraham.lincoln")</f>
@@ -1493,7 +1501,7 @@
     <row r="30" ht="30.75">
       <c r="A30" s="1"/>
       <c r="B30" s="34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
@@ -1553,7 +1561,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="33" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("listDifferences($B$6:$ABB$6, UNIQUE(FILTER(Timecards!$A$1:$A992,Timecards!$C$1:$C992=BurnDoc_project)))"),"")</f>
@@ -1585,7 +1593,7 @@
     </row>
     <row r="33" ht="41.25">
       <c r="B33" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH33" s="19"/>
       <c r="AI33" s="19"/>
@@ -23667,10 +23675,7 @@
       <c r="BB992" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="J6:K11"/>
-    <mergeCell ref="BA6:BB11"/>
-    <mergeCell ref="H6:I6"/>
+  <mergeCells count="9">
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F6:G6"/>
@@ -23678,6 +23683,8 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B32:E32"/>
     <mergeCell ref="B33:C33"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K11"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>